<commit_message>
Agregando ultimos cambios con puesta de datos en master
</commit_message>
<xml_diff>
--- a/Informes_Generats/Informes_Gestió_Desplegament_2023-09-11_2023-09-14.xlsx
+++ b/Informes_Generats/Informes_Gestió_Desplegament_2023-09-11_2023-09-14.xlsx
@@ -190,12 +190,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Resumen'!$A$2:$A$9</f>
+              <f>'Resumen'!$A$2:$A$10</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Resumen'!$B$2:$B$9</f>
+              <f>'Resumen'!$B$2:$B$10</f>
             </numRef>
           </val>
         </ser>
@@ -214,12 +214,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Resumen'!$A$2:$A$9</f>
+              <f>'Resumen'!$A$2:$A$10</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Resumen'!$C$2:$C$9</f>
+              <f>'Resumen'!$C$2:$C$10</f>
             </numRef>
           </val>
         </ser>
@@ -238,12 +238,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Resumen'!$A$2:$A$9</f>
+              <f>'Resumen'!$A$2:$A$10</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Resumen'!$D$2:$D$9</f>
+              <f>'Resumen'!$D$2:$D$10</f>
             </numRef>
           </val>
         </ser>
@@ -629,7 +629,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1771,6 +1771,39 @@
       <c r="G32" s="2" t="inlineStr"/>
       <c r="H32" s="2" t="inlineStr"/>
       <c r="I32" s="3" t="n">
+        <v>45183</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>PRODUCCION</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Mail final. RFC C1642769: Distribucio pegats seguretat anual - 2023</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Pegats</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" s="4" t="n">
         <v>45183</v>
       </c>
     </row>
@@ -1944,7 +1977,7 @@
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Otros</t>
+          <t>Pegats</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -1963,19 +1996,38 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>26</v>
-      </c>
-      <c r="C9" t="n">
+      <c r="B10" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D9" t="n">
-        <v>31</v>
-      </c>
-      <c r="E9" t="n">
+      <c r="D10" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="E10" s="2" t="n">
         <v>9</v>
       </c>
     </row>
@@ -1989,7 +2041,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>De 31 desplegaments, 9 han sigut urgents, d’aquests, 0 tenien incidència associada.</t>
+          <t>De 32 desplegaments, 9 han sigut urgents, d’aquests, 0 tenien incidència associada.</t>
         </is>
       </c>
     </row>

</xml_diff>